<commit_message>
added new scrapped links
</commit_message>
<xml_diff>
--- a/Scrapper/big_five.xlsx
+++ b/Scrapper/big_five.xlsx
@@ -54,7 +54,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,6 +82,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -123,6 +135,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK71"/>
+  <dimension ref="A1:AK72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3516,6 +3530,21 @@
       <c r="AK63" s="6"/>
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>57</v>
+      </c>
+      <c r="B64" s="7">
+        <v>82</v>
+      </c>
+      <c r="C64" s="7">
+        <v>71</v>
+      </c>
+      <c r="D64" s="7">
+        <v>99</v>
+      </c>
+      <c r="E64" s="7">
+        <v>89</v>
+      </c>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
@@ -3549,32 +3578,43 @@
       <c r="AJ64" s="6"/>
       <c r="AK64" s="6"/>
     </row>
-    <row r="65" spans="6:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>69</v>
+      </c>
+      <c r="B65" s="7">
+        <v>84</v>
+      </c>
+      <c r="C65" s="7">
+        <v>95</v>
+      </c>
+      <c r="D65" s="7">
+        <v>109</v>
+      </c>
+      <c r="E65" s="7">
+        <v>77</v>
+      </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
-      <c r="P65" s="6"/>
       <c r="Q65" s="6"/>
       <c r="R65" s="6"/>
       <c r="S65" s="6"/>
       <c r="T65" s="6"/>
       <c r="U65" s="6"/>
       <c r="V65" s="6"/>
-      <c r="W65" s="6"/>
       <c r="X65" s="6"/>
       <c r="Y65" s="6"/>
       <c r="Z65" s="6"/>
       <c r="AA65" s="6"/>
       <c r="AB65" s="6"/>
       <c r="AC65" s="6"/>
-      <c r="AD65" s="6"/>
       <c r="AE65" s="6"/>
       <c r="AF65" s="6"/>
       <c r="AG65" s="6"/>
@@ -3583,32 +3623,43 @@
       <c r="AJ65" s="6"/>
       <c r="AK65" s="6"/>
     </row>
-    <row r="66" spans="6:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
+        <v>73</v>
+      </c>
+      <c r="B66" s="8">
+        <v>99</v>
+      </c>
+      <c r="C66" s="8">
+        <v>101</v>
+      </c>
+      <c r="D66" s="8">
+        <v>86</v>
+      </c>
+      <c r="E66" s="8">
+        <v>100</v>
+      </c>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
-      <c r="P66" s="6"/>
       <c r="Q66" s="6"/>
       <c r="R66" s="6"/>
       <c r="S66" s="6"/>
       <c r="T66" s="6"/>
       <c r="U66" s="6"/>
       <c r="V66" s="6"/>
-      <c r="W66" s="6"/>
       <c r="X66" s="6"/>
       <c r="Y66" s="6"/>
       <c r="Z66" s="6"/>
       <c r="AA66" s="6"/>
       <c r="AB66" s="6"/>
       <c r="AC66" s="6"/>
-      <c r="AD66" s="6"/>
       <c r="AE66" s="6"/>
       <c r="AF66" s="6"/>
       <c r="AG66" s="6"/>
@@ -3617,7 +3668,22 @@
       <c r="AJ66" s="6"/>
       <c r="AK66" s="6"/>
     </row>
-    <row r="67" spans="6:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A67" s="8">
+        <v>53</v>
+      </c>
+      <c r="B67" s="8">
+        <v>104</v>
+      </c>
+      <c r="C67" s="8">
+        <v>93</v>
+      </c>
+      <c r="D67" s="8">
+        <v>104</v>
+      </c>
+      <c r="E67" s="8">
+        <v>83</v>
+      </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
@@ -3651,7 +3717,22 @@
       <c r="AJ67" s="6"/>
       <c r="AK67" s="6"/>
     </row>
-    <row r="68" spans="6:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A68" s="8">
+        <v>48</v>
+      </c>
+      <c r="B68" s="8">
+        <v>75</v>
+      </c>
+      <c r="C68" s="8">
+        <v>94</v>
+      </c>
+      <c r="D68" s="8">
+        <v>86</v>
+      </c>
+      <c r="E68" s="8">
+        <v>72</v>
+      </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
@@ -3685,7 +3766,22 @@
       <c r="AJ68" s="6"/>
       <c r="AK68" s="6"/>
     </row>
-    <row r="69" spans="6:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A69" s="8">
+        <v>71</v>
+      </c>
+      <c r="B69" s="8">
+        <v>77</v>
+      </c>
+      <c r="C69" s="8">
+        <v>87</v>
+      </c>
+      <c r="D69" s="8">
+        <v>97</v>
+      </c>
+      <c r="E69" s="8">
+        <v>95</v>
+      </c>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
@@ -3719,7 +3815,22 @@
       <c r="AJ69" s="6"/>
       <c r="AK69" s="6"/>
     </row>
-    <row r="70" spans="6:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A70" s="8">
+        <v>64</v>
+      </c>
+      <c r="B70" s="8">
+        <v>91</v>
+      </c>
+      <c r="C70" s="8">
+        <v>97</v>
+      </c>
+      <c r="D70" s="8">
+        <v>92</v>
+      </c>
+      <c r="E70" s="8">
+        <v>86</v>
+      </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
@@ -3753,7 +3864,22 @@
       <c r="AJ70" s="6"/>
       <c r="AK70" s="6"/>
     </row>
-    <row r="71" spans="6:37" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A71" s="8">
+        <v>54</v>
+      </c>
+      <c r="B71" s="8">
+        <v>68</v>
+      </c>
+      <c r="C71" s="8">
+        <v>80</v>
+      </c>
+      <c r="D71" s="8">
+        <v>82</v>
+      </c>
+      <c r="E71" s="8">
+        <v>94</v>
+      </c>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
@@ -3787,6 +3913,23 @@
       <c r="AJ71" s="6"/>
       <c r="AK71" s="6"/>
     </row>
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A72" s="8">
+        <v>58</v>
+      </c>
+      <c r="B72" s="8">
+        <v>73</v>
+      </c>
+      <c r="C72" s="8">
+        <v>95</v>
+      </c>
+      <c r="D72" s="8">
+        <v>104</v>
+      </c>
+      <c r="E72" s="8">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
modified order in big_five data
</commit_message>
<xml_diff>
--- a/Scrapper/big_five.xlsx
+++ b/Scrapper/big_five.xlsx
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E72"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,20 +2256,20 @@
       <c r="AK37" s="6"/>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>93</v>
-      </c>
-      <c r="B38" s="4">
-        <v>96</v>
-      </c>
-      <c r="C38" s="4">
-        <v>97</v>
-      </c>
-      <c r="D38" s="4">
-        <v>80</v>
-      </c>
-      <c r="E38" s="4">
-        <v>54</v>
+      <c r="A38" s="7">
+        <v>57</v>
+      </c>
+      <c r="B38" s="7">
+        <v>82</v>
+      </c>
+      <c r="C38" s="7">
+        <v>71</v>
+      </c>
+      <c r="D38" s="7">
+        <v>99</v>
+      </c>
+      <c r="E38" s="7">
+        <v>89</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -2305,20 +2305,20 @@
       <c r="AK38" s="6"/>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>68</v>
-      </c>
-      <c r="B39" s="4">
-        <v>71</v>
-      </c>
-      <c r="C39" s="4">
-        <v>65</v>
-      </c>
-      <c r="D39" s="4">
-        <v>99</v>
-      </c>
-      <c r="E39" s="4">
-        <v>114</v>
+      <c r="A39" s="7">
+        <v>69</v>
+      </c>
+      <c r="B39" s="7">
+        <v>84</v>
+      </c>
+      <c r="C39" s="7">
+        <v>95</v>
+      </c>
+      <c r="D39" s="7">
+        <v>109</v>
+      </c>
+      <c r="E39" s="7">
+        <v>77</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -2355,19 +2355,19 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B40" s="4">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40" s="4">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="D40" s="4">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E40" s="4">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -2404,19 +2404,19 @@
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B41" s="4">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C41" s="4">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D41" s="4">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E41" s="4">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -2453,19 +2453,19 @@
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B42" s="4">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C42" s="4">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D42" s="4">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E42" s="4">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -2502,19 +2502,19 @@
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B43" s="4">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="C43" s="4">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D43" s="4">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E43" s="4">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -2554,16 +2554,16 @@
         <v>74</v>
       </c>
       <c r="B44" s="4">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C44" s="4">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="D44" s="4">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E44" s="4">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -2600,19 +2600,19 @@
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B45" s="4">
         <v>96</v>
       </c>
       <c r="C45" s="4">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D45" s="4">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E45" s="4">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -2649,19 +2649,19 @@
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B46" s="4">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C46" s="4">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D46" s="4">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E46" s="4">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -2698,19 +2698,19 @@
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B47" s="4">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C47" s="4">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D47" s="4">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E47" s="4">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -2747,19 +2747,19 @@
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B48" s="4">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C48" s="4">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D48" s="4">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E48" s="4">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -2796,19 +2796,19 @@
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B49" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C49" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D49" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E49" s="4">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -2845,19 +2845,19 @@
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B50" s="4">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C50" s="4">
         <v>93</v>
       </c>
       <c r="D50" s="4">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E50" s="4">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -2894,19 +2894,19 @@
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B51" s="4">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C51" s="4">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D51" s="4">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E51" s="4">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -2943,19 +2943,19 @@
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="B52" s="4">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="C52" s="4">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D52" s="4">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E52" s="4">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
@@ -2992,19 +2992,19 @@
     </row>
     <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="B53" s="4">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C53" s="4">
         <v>78</v>
       </c>
       <c r="D53" s="4">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E53" s="4">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -3040,20 +3040,20 @@
       <c r="AK53" s="6"/>
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
-        <v>70</v>
-      </c>
-      <c r="B54" s="5">
-        <v>85</v>
-      </c>
-      <c r="C54" s="5">
-        <v>69</v>
-      </c>
-      <c r="D54" s="5">
-        <v>98</v>
-      </c>
-      <c r="E54" s="5">
-        <v>91</v>
+      <c r="A54" s="4">
+        <v>56</v>
+      </c>
+      <c r="B54" s="4">
+        <v>102</v>
+      </c>
+      <c r="C54" s="4">
+        <v>77</v>
+      </c>
+      <c r="D54" s="4">
+        <v>82</v>
+      </c>
+      <c r="E54" s="4">
+        <v>105</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -3089,20 +3089,20 @@
       <c r="AK54" s="6"/>
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
-        <v>89</v>
-      </c>
-      <c r="B55" s="5">
-        <v>60</v>
-      </c>
-      <c r="C55" s="5">
-        <v>80</v>
-      </c>
-      <c r="D55" s="5">
-        <v>73</v>
-      </c>
-      <c r="E55" s="5">
-        <v>55</v>
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4">
+        <v>82</v>
+      </c>
+      <c r="C55" s="4">
+        <v>78</v>
+      </c>
+      <c r="D55" s="4">
+        <v>107</v>
+      </c>
+      <c r="E55" s="4">
+        <v>103</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
@@ -3138,20 +3138,20 @@
       <c r="AK55" s="6"/>
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
-        <v>52</v>
-      </c>
-      <c r="B56" s="5">
-        <v>76</v>
-      </c>
-      <c r="C56" s="5">
-        <v>68</v>
-      </c>
-      <c r="D56" s="5">
-        <v>96</v>
-      </c>
-      <c r="E56" s="5">
-        <v>102</v>
+      <c r="A56" s="8">
+        <v>73</v>
+      </c>
+      <c r="B56" s="8">
+        <v>99</v>
+      </c>
+      <c r="C56" s="8">
+        <v>101</v>
+      </c>
+      <c r="D56" s="8">
+        <v>86</v>
+      </c>
+      <c r="E56" s="8">
+        <v>100</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -3187,20 +3187,20 @@
       <c r="AK56" s="6"/>
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
-        <v>61</v>
-      </c>
-      <c r="B57" s="5">
-        <v>94</v>
-      </c>
-      <c r="C57" s="5">
-        <v>95</v>
-      </c>
-      <c r="D57" s="5">
-        <v>98</v>
-      </c>
-      <c r="E57" s="5">
-        <v>88</v>
+      <c r="A57" s="8">
+        <v>53</v>
+      </c>
+      <c r="B57" s="8">
+        <v>104</v>
+      </c>
+      <c r="C57" s="8">
+        <v>93</v>
+      </c>
+      <c r="D57" s="8">
+        <v>104</v>
+      </c>
+      <c r="E57" s="8">
+        <v>83</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
@@ -3236,20 +3236,20 @@
       <c r="AK57" s="6"/>
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
+      <c r="A58" s="8">
+        <v>48</v>
+      </c>
+      <c r="B58" s="8">
+        <v>75</v>
+      </c>
+      <c r="C58" s="8">
+        <v>94</v>
+      </c>
+      <c r="D58" s="8">
+        <v>86</v>
+      </c>
+      <c r="E58" s="8">
         <v>72</v>
-      </c>
-      <c r="B58" s="5">
-        <v>77</v>
-      </c>
-      <c r="C58" s="5">
-        <v>100</v>
-      </c>
-      <c r="D58" s="5">
-        <v>83</v>
-      </c>
-      <c r="E58" s="5">
-        <v>105</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
@@ -3285,20 +3285,20 @@
       <c r="AK58" s="6"/>
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
-        <v>67</v>
-      </c>
-      <c r="B59" s="5">
-        <v>76</v>
-      </c>
-      <c r="C59" s="5">
-        <v>82</v>
-      </c>
-      <c r="D59" s="5">
-        <v>78</v>
-      </c>
-      <c r="E59" s="5">
-        <v>98</v>
+      <c r="A59" s="8">
+        <v>71</v>
+      </c>
+      <c r="B59" s="8">
+        <v>77</v>
+      </c>
+      <c r="C59" s="8">
+        <v>87</v>
+      </c>
+      <c r="D59" s="8">
+        <v>97</v>
+      </c>
+      <c r="E59" s="8">
+        <v>95</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
@@ -3334,20 +3334,20 @@
       <c r="AK59" s="6"/>
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
-        <v>62</v>
-      </c>
-      <c r="B60" s="5">
-        <v>83</v>
-      </c>
-      <c r="C60" s="5">
-        <v>78</v>
-      </c>
-      <c r="D60" s="5">
-        <v>100</v>
-      </c>
-      <c r="E60" s="5">
-        <v>110</v>
+      <c r="A60" s="8">
+        <v>64</v>
+      </c>
+      <c r="B60" s="8">
+        <v>91</v>
+      </c>
+      <c r="C60" s="8">
+        <v>97</v>
+      </c>
+      <c r="D60" s="8">
+        <v>92</v>
+      </c>
+      <c r="E60" s="8">
+        <v>86</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -3383,20 +3383,20 @@
       <c r="AK60" s="6"/>
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <v>77</v>
-      </c>
-      <c r="B61" s="5">
-        <v>73</v>
-      </c>
-      <c r="C61" s="5">
+      <c r="A61" s="8">
+        <v>54</v>
+      </c>
+      <c r="B61" s="8">
+        <v>68</v>
+      </c>
+      <c r="C61" s="8">
         <v>80</v>
       </c>
-      <c r="D61" s="5">
-        <v>100</v>
-      </c>
-      <c r="E61" s="5">
-        <v>89</v>
+      <c r="D61" s="8">
+        <v>82</v>
+      </c>
+      <c r="E61" s="8">
+        <v>94</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -3432,19 +3432,19 @@
       <c r="AK61" s="6"/>
     </row>
     <row r="62" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
-        <v>68</v>
-      </c>
-      <c r="B62" s="5">
-        <v>76</v>
-      </c>
-      <c r="C62" s="5">
-        <v>82</v>
-      </c>
-      <c r="D62" s="5">
+      <c r="A62" s="8">
+        <v>58</v>
+      </c>
+      <c r="B62" s="8">
+        <v>73</v>
+      </c>
+      <c r="C62" s="8">
         <v>95</v>
       </c>
-      <c r="E62" s="5">
+      <c r="D62" s="8">
+        <v>104</v>
+      </c>
+      <c r="E62" s="8">
         <v>89</v>
       </c>
       <c r="F62" s="6"/>
@@ -3482,19 +3482,19 @@
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B63" s="5">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C63" s="5">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="D63" s="5">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E63" s="5">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -3530,20 +3530,20 @@
       <c r="AK63" s="6"/>
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A64" s="7">
-        <v>57</v>
-      </c>
-      <c r="B64" s="7">
-        <v>82</v>
-      </c>
-      <c r="C64" s="7">
-        <v>71</v>
-      </c>
-      <c r="D64" s="7">
-        <v>99</v>
-      </c>
-      <c r="E64" s="7">
+      <c r="A64" s="5">
         <v>89</v>
+      </c>
+      <c r="B64" s="5">
+        <v>60</v>
+      </c>
+      <c r="C64" s="5">
+        <v>80</v>
+      </c>
+      <c r="D64" s="5">
+        <v>73</v>
+      </c>
+      <c r="E64" s="5">
+        <v>55</v>
       </c>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
@@ -3579,20 +3579,20 @@
       <c r="AK64" s="6"/>
     </row>
     <row r="65" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A65" s="7">
-        <v>69</v>
-      </c>
-      <c r="B65" s="7">
-        <v>84</v>
-      </c>
-      <c r="C65" s="7">
-        <v>95</v>
-      </c>
-      <c r="D65" s="7">
-        <v>109</v>
-      </c>
-      <c r="E65" s="7">
-        <v>77</v>
+      <c r="A65" s="5">
+        <v>52</v>
+      </c>
+      <c r="B65" s="5">
+        <v>76</v>
+      </c>
+      <c r="C65" s="5">
+        <v>68</v>
+      </c>
+      <c r="D65" s="5">
+        <v>96</v>
+      </c>
+      <c r="E65" s="5">
+        <v>102</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
@@ -3624,20 +3624,20 @@
       <c r="AK65" s="6"/>
     </row>
     <row r="66" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A66" s="8">
-        <v>73</v>
-      </c>
-      <c r="B66" s="8">
-        <v>99</v>
-      </c>
-      <c r="C66" s="8">
-        <v>101</v>
-      </c>
-      <c r="D66" s="8">
-        <v>86</v>
-      </c>
-      <c r="E66" s="8">
-        <v>100</v>
+      <c r="A66" s="5">
+        <v>61</v>
+      </c>
+      <c r="B66" s="5">
+        <v>94</v>
+      </c>
+      <c r="C66" s="5">
+        <v>95</v>
+      </c>
+      <c r="D66" s="5">
+        <v>98</v>
+      </c>
+      <c r="E66" s="5">
+        <v>88</v>
       </c>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
@@ -3669,20 +3669,20 @@
       <c r="AK66" s="6"/>
     </row>
     <row r="67" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A67" s="8">
-        <v>53</v>
-      </c>
-      <c r="B67" s="8">
-        <v>104</v>
-      </c>
-      <c r="C67" s="8">
-        <v>93</v>
-      </c>
-      <c r="D67" s="8">
-        <v>104</v>
-      </c>
-      <c r="E67" s="8">
+      <c r="A67" s="5">
+        <v>72</v>
+      </c>
+      <c r="B67" s="5">
+        <v>77</v>
+      </c>
+      <c r="C67" s="5">
+        <v>100</v>
+      </c>
+      <c r="D67" s="5">
         <v>83</v>
+      </c>
+      <c r="E67" s="5">
+        <v>105</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
@@ -3718,20 +3718,20 @@
       <c r="AK67" s="6"/>
     </row>
     <row r="68" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A68" s="8">
-        <v>48</v>
-      </c>
-      <c r="B68" s="8">
-        <v>75</v>
-      </c>
-      <c r="C68" s="8">
-        <v>94</v>
-      </c>
-      <c r="D68" s="8">
-        <v>86</v>
-      </c>
-      <c r="E68" s="8">
-        <v>72</v>
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="5">
+        <v>76</v>
+      </c>
+      <c r="C68" s="5">
+        <v>82</v>
+      </c>
+      <c r="D68" s="5">
+        <v>78</v>
+      </c>
+      <c r="E68" s="5">
+        <v>98</v>
       </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
@@ -3767,20 +3767,20 @@
       <c r="AK68" s="6"/>
     </row>
     <row r="69" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A69" s="8">
-        <v>71</v>
-      </c>
-      <c r="B69" s="8">
-        <v>77</v>
-      </c>
-      <c r="C69" s="8">
-        <v>87</v>
-      </c>
-      <c r="D69" s="8">
-        <v>97</v>
-      </c>
-      <c r="E69" s="8">
-        <v>95</v>
+      <c r="A69" s="5">
+        <v>62</v>
+      </c>
+      <c r="B69" s="5">
+        <v>83</v>
+      </c>
+      <c r="C69" s="5">
+        <v>78</v>
+      </c>
+      <c r="D69" s="5">
+        <v>100</v>
+      </c>
+      <c r="E69" s="5">
+        <v>110</v>
       </c>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
@@ -3816,20 +3816,20 @@
       <c r="AK69" s="6"/>
     </row>
     <row r="70" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A70" s="8">
-        <v>64</v>
-      </c>
-      <c r="B70" s="8">
-        <v>91</v>
-      </c>
-      <c r="C70" s="8">
-        <v>97</v>
-      </c>
-      <c r="D70" s="8">
-        <v>92</v>
-      </c>
-      <c r="E70" s="8">
-        <v>86</v>
+      <c r="A70" s="5">
+        <v>77</v>
+      </c>
+      <c r="B70" s="5">
+        <v>73</v>
+      </c>
+      <c r="C70" s="5">
+        <v>80</v>
+      </c>
+      <c r="D70" s="5">
+        <v>100</v>
+      </c>
+      <c r="E70" s="5">
+        <v>89</v>
       </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
@@ -3865,20 +3865,20 @@
       <c r="AK70" s="6"/>
     </row>
     <row r="71" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
-        <v>54</v>
-      </c>
-      <c r="B71" s="8">
+      <c r="A71" s="5">
         <v>68</v>
       </c>
-      <c r="C71" s="8">
-        <v>80</v>
-      </c>
-      <c r="D71" s="8">
+      <c r="B71" s="5">
+        <v>76</v>
+      </c>
+      <c r="C71" s="5">
         <v>82</v>
       </c>
-      <c r="E71" s="8">
-        <v>94</v>
+      <c r="D71" s="5">
+        <v>95</v>
+      </c>
+      <c r="E71" s="5">
+        <v>89</v>
       </c>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
@@ -3914,20 +3914,20 @@
       <c r="AK71" s="6"/>
     </row>
     <row r="72" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A72" s="8">
-        <v>58</v>
-      </c>
-      <c r="B72" s="8">
-        <v>73</v>
-      </c>
-      <c r="C72" s="8">
-        <v>95</v>
-      </c>
-      <c r="D72" s="8">
-        <v>104</v>
-      </c>
-      <c r="E72" s="8">
-        <v>89</v>
+      <c r="A72" s="5">
+        <v>52</v>
+      </c>
+      <c r="B72" s="5">
+        <v>84</v>
+      </c>
+      <c r="C72" s="5">
+        <v>88</v>
+      </c>
+      <c r="D72" s="5">
+        <v>92</v>
+      </c>
+      <c r="E72" s="5">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>